<commit_message>
MAJ cahier des charges et liste de composants
</commit_message>
<xml_diff>
--- a/Liste de composant KANE KANIA MARTIN.xlsx
+++ b/Liste de composant KANE KANIA MARTIN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet IUT\SAE-S5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IUT\SAE-S5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE385F63-F209-4608-A46C-2282B3659B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D090349C-57E2-4376-B56D-1C207DC6ABD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D77634F6-E77F-462F-9E70-584C282198EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{D77634F6-E77F-462F-9E70-584C282198EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -53,10 +53,10 @@
     <t>ESP32 S3-Devkit C</t>
   </si>
   <si>
-    <t xml:space="preserve">Raspberry pi </t>
-  </si>
-  <si>
-    <t>https://www.kubii.com/fr/cartes-nano-ordinateurs/1401-raspberry-pi-zero-v13-kubii-3272496006973.html?gad_source=1</t>
+    <t>Bobine de filament PLA Matte Noir</t>
+  </si>
+  <si>
+    <t>https://eu.store.bambulab.com/fr-fr/collections/all/products/pla-matte-filament?variant=42996742750427</t>
   </si>
 </sst>
 </file>
@@ -110,7 +110,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -446,17 +446,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -478,12 +478,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>12.9</v>
+        <v>23.18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -492,9 +492,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{56C8FB96-6923-4D7B-9CFB-9CBDECB8C1FB}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{DF772A78-3A31-4F37-B918-28B7BC5A1011}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>